<commit_message>
added folders, updated data.xlsx
</commit_message>
<xml_diff>
--- a/data.xlsx
+++ b/data.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Projects\CertIssue\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1FB862E5-B153-49CB-B0BA-BFBAA261C560}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CCBF6979-E405-476E-8CB6-F42202C9C1D2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{4DB77375-516C-4A49-9364-A556AA4238B8}"/>
   </bookViews>
@@ -260,10 +260,10 @@
     <t>0x2F0F1f694C37c390ce3025Ff2862E65e70CAE62C</t>
   </si>
   <si>
-    <t>[</t>
-  </si>
-  <si>
     <t>]</t>
+  </si>
+  <si>
+    <t>user_data = [</t>
   </si>
 </sst>
 </file>
@@ -466,10 +466,10 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="7" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="5" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -787,7 +787,7 @@
   <dimension ref="A1:F33"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K4" sqref="K4"/>
+      <selection activeCell="F1" sqref="F1:F33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="26.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -811,8 +811,8 @@
       <c r="D1" s="6" t="s">
         <v>1</v>
       </c>
-      <c r="F1" s="13" t="s">
-        <v>75</v>
+      <c r="F1" s="14" t="s">
+        <v>76</v>
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.25">
@@ -828,7 +828,7 @@
       <c r="D2" s="9" t="s">
         <v>66</v>
       </c>
-      <c r="F2" s="14" t="str">
+      <c r="F2" s="13" t="str">
         <f>"{ 'tournament_name': '"&amp;B2&amp;"', 'user_name': '"&amp;C2&amp;"', 'user_account': '"&amp;D2&amp;"'},"</f>
         <v>{ 'tournament_name': 'Tournament 1', 'user_name': 'User 1', 'user_account': '0x9E6407D973648A3382B8E84e92E1BD3DFD2E9387'},</v>
       </c>
@@ -847,7 +847,7 @@
       <c r="D3" s="9" t="s">
         <v>67</v>
       </c>
-      <c r="F3" s="14" t="str">
+      <c r="F3" s="13" t="str">
         <f t="shared" ref="F3:F32" si="0">"{ 'tournament_name': '"&amp;B3&amp;"', 'user_name': '"&amp;C3&amp;"', 'user_account': '"&amp;D3&amp;"'},"</f>
         <v>{ 'tournament_name': 'Tournament 2', 'user_name': 'User 2', 'user_account': '0x971AaCB8CC05Dfea0D71Ca62C4e47C0F0dda5B97'},</v>
       </c>
@@ -866,7 +866,7 @@
       <c r="D4" s="9" t="s">
         <v>68</v>
       </c>
-      <c r="F4" s="14" t="str">
+      <c r="F4" s="13" t="str">
         <f t="shared" si="0"/>
         <v>{ 'tournament_name': 'Tournament 3', 'user_name': 'User 3', 'user_account': '0xCa24dAe560a0B628408FB323B5C7ec0B03276F1d'},</v>
       </c>
@@ -885,7 +885,7 @@
       <c r="D5" s="9" t="s">
         <v>69</v>
       </c>
-      <c r="F5" s="14" t="str">
+      <c r="F5" s="13" t="str">
         <f t="shared" si="0"/>
         <v>{ 'tournament_name': 'Tournament 4', 'user_name': 'User 4', 'user_account': '0xbb141b9A5b96440d651Bcd9C29EF9A0a77300bC0'},</v>
       </c>
@@ -904,7 +904,7 @@
       <c r="D6" s="9" t="s">
         <v>70</v>
       </c>
-      <c r="F6" s="14" t="str">
+      <c r="F6" s="13" t="str">
         <f t="shared" si="0"/>
         <v>{ 'tournament_name': 'Tournament 5', 'user_name': 'User 5', 'user_account': '0xf5a34486b08300F426432b035BE949e2AF1aC375'},</v>
       </c>
@@ -923,7 +923,7 @@
       <c r="D7" s="9" t="s">
         <v>71</v>
       </c>
-      <c r="F7" s="14" t="str">
+      <c r="F7" s="13" t="str">
         <f t="shared" si="0"/>
         <v>{ 'tournament_name': 'Tournament 6', 'user_name': 'User 6', 'user_account': '0x35cbf3b391872032C2f8bfB67c0f9A2FeFc46508'},</v>
       </c>
@@ -942,7 +942,7 @@
       <c r="D8" s="9" t="s">
         <v>72</v>
       </c>
-      <c r="F8" s="14" t="str">
+      <c r="F8" s="13" t="str">
         <f t="shared" si="0"/>
         <v>{ 'tournament_name': 'Tournament 7', 'user_name': 'User 7', 'user_account': '0x8071bCe7d344D607213512BE9dcBD6BC756B11E7'},</v>
       </c>
@@ -961,7 +961,7 @@
       <c r="D9" s="9" t="s">
         <v>73</v>
       </c>
-      <c r="F9" s="14" t="str">
+      <c r="F9" s="13" t="str">
         <f t="shared" si="0"/>
         <v>{ 'tournament_name': 'Tournament 8', 'user_name': 'User 8', 'user_account': '0xCA3aEF4A1755Ec7c6c7170f4Bf665d1f94167E62'},</v>
       </c>
@@ -980,7 +980,7 @@
       <c r="D10" s="9" t="s">
         <v>74</v>
       </c>
-      <c r="F10" s="14" t="str">
+      <c r="F10" s="13" t="str">
         <f t="shared" si="0"/>
         <v>{ 'tournament_name': 'Tournament 9', 'user_name': 'User 9', 'user_account': '0x2F0F1f694C37c390ce3025Ff2862E65e70CAE62C'},</v>
       </c>
@@ -999,7 +999,7 @@
       <c r="D11" s="9" t="s">
         <v>66</v>
       </c>
-      <c r="F11" s="14" t="str">
+      <c r="F11" s="13" t="str">
         <f t="shared" si="0"/>
         <v>{ 'tournament_name': 'Tournament 10', 'user_name': 'User 10', 'user_account': '0x9E6407D973648A3382B8E84e92E1BD3DFD2E9387'},</v>
       </c>
@@ -1018,7 +1018,7 @@
       <c r="D12" s="9" t="s">
         <v>67</v>
       </c>
-      <c r="F12" s="14" t="str">
+      <c r="F12" s="13" t="str">
         <f t="shared" si="0"/>
         <v>{ 'tournament_name': 'Tournament 11', 'user_name': 'User 11', 'user_account': '0x971AaCB8CC05Dfea0D71Ca62C4e47C0F0dda5B97'},</v>
       </c>
@@ -1037,7 +1037,7 @@
       <c r="D13" s="9" t="s">
         <v>68</v>
       </c>
-      <c r="F13" s="14" t="str">
+      <c r="F13" s="13" t="str">
         <f t="shared" si="0"/>
         <v>{ 'tournament_name': 'Tournament 12', 'user_name': 'User 12', 'user_account': '0xCa24dAe560a0B628408FB323B5C7ec0B03276F1d'},</v>
       </c>
@@ -1056,7 +1056,7 @@
       <c r="D14" s="9" t="s">
         <v>69</v>
       </c>
-      <c r="F14" s="14" t="str">
+      <c r="F14" s="13" t="str">
         <f t="shared" si="0"/>
         <v>{ 'tournament_name': 'Tournament 13', 'user_name': 'User 13', 'user_account': '0xbb141b9A5b96440d651Bcd9C29EF9A0a77300bC0'},</v>
       </c>
@@ -1075,7 +1075,7 @@
       <c r="D15" s="9" t="s">
         <v>70</v>
       </c>
-      <c r="F15" s="14" t="str">
+      <c r="F15" s="13" t="str">
         <f t="shared" si="0"/>
         <v>{ 'tournament_name': 'Tournament 14', 'user_name': 'User 14', 'user_account': '0xf5a34486b08300F426432b035BE949e2AF1aC375'},</v>
       </c>
@@ -1094,7 +1094,7 @@
       <c r="D16" s="9" t="s">
         <v>71</v>
       </c>
-      <c r="F16" s="14" t="str">
+      <c r="F16" s="13" t="str">
         <f t="shared" si="0"/>
         <v>{ 'tournament_name': 'Tournament 15', 'user_name': 'User 15', 'user_account': '0x35cbf3b391872032C2f8bfB67c0f9A2FeFc46508'},</v>
       </c>
@@ -1113,7 +1113,7 @@
       <c r="D17" s="9" t="s">
         <v>72</v>
       </c>
-      <c r="F17" s="14" t="str">
+      <c r="F17" s="13" t="str">
         <f t="shared" si="0"/>
         <v>{ 'tournament_name': 'Tournament 16', 'user_name': 'User 16', 'user_account': '0x8071bCe7d344D607213512BE9dcBD6BC756B11E7'},</v>
       </c>
@@ -1132,7 +1132,7 @@
       <c r="D18" s="9" t="s">
         <v>73</v>
       </c>
-      <c r="F18" s="14" t="str">
+      <c r="F18" s="13" t="str">
         <f t="shared" si="0"/>
         <v>{ 'tournament_name': 'Tournament 17', 'user_name': 'User 17', 'user_account': '0xCA3aEF4A1755Ec7c6c7170f4Bf665d1f94167E62'},</v>
       </c>
@@ -1151,7 +1151,7 @@
       <c r="D19" s="9" t="s">
         <v>74</v>
       </c>
-      <c r="F19" s="14" t="str">
+      <c r="F19" s="13" t="str">
         <f t="shared" si="0"/>
         <v>{ 'tournament_name': 'Tournament 18', 'user_name': 'User 18', 'user_account': '0x2F0F1f694C37c390ce3025Ff2862E65e70CAE62C'},</v>
       </c>
@@ -1170,7 +1170,7 @@
       <c r="D20" s="9" t="s">
         <v>66</v>
       </c>
-      <c r="F20" s="14" t="str">
+      <c r="F20" s="13" t="str">
         <f t="shared" si="0"/>
         <v>{ 'tournament_name': 'Tournament 19', 'user_name': 'User 19', 'user_account': '0x9E6407D973648A3382B8E84e92E1BD3DFD2E9387'},</v>
       </c>
@@ -1189,7 +1189,7 @@
       <c r="D21" s="9" t="s">
         <v>67</v>
       </c>
-      <c r="F21" s="14" t="str">
+      <c r="F21" s="13" t="str">
         <f t="shared" si="0"/>
         <v>{ 'tournament_name': 'Tournament 20', 'user_name': 'User 20', 'user_account': '0x971AaCB8CC05Dfea0D71Ca62C4e47C0F0dda5B97'},</v>
       </c>
@@ -1208,7 +1208,7 @@
       <c r="D22" s="9" t="s">
         <v>68</v>
       </c>
-      <c r="F22" s="14" t="str">
+      <c r="F22" s="13" t="str">
         <f t="shared" si="0"/>
         <v>{ 'tournament_name': 'Tournament 21', 'user_name': 'User 21', 'user_account': '0xCa24dAe560a0B628408FB323B5C7ec0B03276F1d'},</v>
       </c>
@@ -1227,7 +1227,7 @@
       <c r="D23" s="9" t="s">
         <v>69</v>
       </c>
-      <c r="F23" s="14" t="str">
+      <c r="F23" s="13" t="str">
         <f t="shared" si="0"/>
         <v>{ 'tournament_name': 'Tournament 22', 'user_name': 'User 22', 'user_account': '0xbb141b9A5b96440d651Bcd9C29EF9A0a77300bC0'},</v>
       </c>
@@ -1246,7 +1246,7 @@
       <c r="D24" s="9" t="s">
         <v>70</v>
       </c>
-      <c r="F24" s="14" t="str">
+      <c r="F24" s="13" t="str">
         <f t="shared" si="0"/>
         <v>{ 'tournament_name': 'Tournament 23', 'user_name': 'User 23', 'user_account': '0xf5a34486b08300F426432b035BE949e2AF1aC375'},</v>
       </c>
@@ -1265,7 +1265,7 @@
       <c r="D25" s="9" t="s">
         <v>71</v>
       </c>
-      <c r="F25" s="14" t="str">
+      <c r="F25" s="13" t="str">
         <f t="shared" si="0"/>
         <v>{ 'tournament_name': 'Tournament 24', 'user_name': 'User 24', 'user_account': '0x35cbf3b391872032C2f8bfB67c0f9A2FeFc46508'},</v>
       </c>
@@ -1284,7 +1284,7 @@
       <c r="D26" s="9" t="s">
         <v>72</v>
       </c>
-      <c r="F26" s="14" t="str">
+      <c r="F26" s="13" t="str">
         <f t="shared" si="0"/>
         <v>{ 'tournament_name': 'Tournament 25', 'user_name': 'User 25', 'user_account': '0x8071bCe7d344D607213512BE9dcBD6BC756B11E7'},</v>
       </c>
@@ -1303,7 +1303,7 @@
       <c r="D27" s="9" t="s">
         <v>73</v>
       </c>
-      <c r="F27" s="14" t="str">
+      <c r="F27" s="13" t="str">
         <f t="shared" si="0"/>
         <v>{ 'tournament_name': 'Tournament 26', 'user_name': 'User 26', 'user_account': '0xCA3aEF4A1755Ec7c6c7170f4Bf665d1f94167E62'},</v>
       </c>
@@ -1322,7 +1322,7 @@
       <c r="D28" s="9" t="s">
         <v>74</v>
       </c>
-      <c r="F28" s="14" t="str">
+      <c r="F28" s="13" t="str">
         <f t="shared" si="0"/>
         <v>{ 'tournament_name': 'Tournament 27', 'user_name': 'User 27', 'user_account': '0x2F0F1f694C37c390ce3025Ff2862E65e70CAE62C'},</v>
       </c>
@@ -1342,7 +1342,7 @@
         <f>D26</f>
         <v>0x8071bCe7d344D607213512BE9dcBD6BC756B11E7</v>
       </c>
-      <c r="F29" s="14" t="str">
+      <c r="F29" s="13" t="str">
         <f t="shared" si="0"/>
         <v>{ 'tournament_name': 'Tournament 28', 'user_name': 'User 28', 'user_account': '0x8071bCe7d344D607213512BE9dcBD6BC756B11E7'},</v>
       </c>
@@ -1362,7 +1362,7 @@
         <f>D27</f>
         <v>0xCA3aEF4A1755Ec7c6c7170f4Bf665d1f94167E62</v>
       </c>
-      <c r="F30" s="14" t="str">
+      <c r="F30" s="13" t="str">
         <f t="shared" si="0"/>
         <v>{ 'tournament_name': 'Tournament 29', 'user_name': 'User 29', 'user_account': '0xCA3aEF4A1755Ec7c6c7170f4Bf665d1f94167E62'},</v>
       </c>
@@ -1382,7 +1382,7 @@
         <f>D28</f>
         <v>0x2F0F1f694C37c390ce3025Ff2862E65e70CAE62C</v>
       </c>
-      <c r="F31" s="14" t="str">
+      <c r="F31" s="13" t="str">
         <f t="shared" si="0"/>
         <v>{ 'tournament_name': 'Tournament 30', 'user_name': 'User 30', 'user_account': '0x2F0F1f694C37c390ce3025Ff2862E65e70CAE62C'},</v>
       </c>
@@ -1402,14 +1402,14 @@
         <f>D23</f>
         <v>0xbb141b9A5b96440d651Bcd9C29EF9A0a77300bC0</v>
       </c>
-      <c r="F32" s="14" t="str">
+      <c r="F32" s="13" t="str">
         <f t="shared" si="0"/>
         <v>{ 'tournament_name': 'Tournament 31', 'user_name': 'User 31', 'user_account': '0xbb141b9A5b96440d651Bcd9C29EF9A0a77300bC0'},</v>
       </c>
     </row>
     <row r="33" spans="6:6" x14ac:dyDescent="0.25">
-      <c r="F33" s="14" t="s">
-        <v>76</v>
+      <c r="F33" s="13" t="s">
+        <v>75</v>
       </c>
     </row>
   </sheetData>

</xml_diff>